<commit_message>
csvs of unique variable names
</commit_message>
<xml_diff>
--- a/Excel/hh_vars_tokeep.xlsx
+++ b/Excel/hh_vars_tokeep.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8161" uniqueCount="3032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8164" uniqueCount="3035">
   <si>
     <t>var</t>
   </si>
@@ -9115,6 +9115,15 @@
   </si>
   <si>
     <t>share_toilet</t>
+  </si>
+  <si>
+    <t>cooking_fuel</t>
+  </si>
+  <si>
+    <t>mosquito_net</t>
+  </si>
+  <si>
+    <t>use_mosquito_net</t>
   </si>
 </sst>
 </file>
@@ -9485,14 +9494,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2713"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7.1640625" customWidth="1"/>
     <col min="3" max="3" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -10591,6 +10601,9 @@
       <c r="E61">
         <v>60</v>
       </c>
+      <c r="F61" t="s">
+        <v>3032</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
@@ -10608,6 +10621,9 @@
       <c r="E62">
         <v>61</v>
       </c>
+      <c r="F62" t="s">
+        <v>3033</v>
+      </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
@@ -10624,6 +10640,9 @@
       </c>
       <c r="E63">
         <v>62</v>
+      </c>
+      <c r="F63" t="s">
+        <v>3034</v>
       </c>
     </row>
     <row r="64" spans="1:6">

</xml_diff>

<commit_message>
Add some more variables to keep
</commit_message>
<xml_diff>
--- a/Excel/hh_vars_tokeep.xlsx
+++ b/Excel/hh_vars_tokeep.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="1065" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1065" windowWidth="15105" windowHeight="6885" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="hh_labels.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4737" uniqueCount="2670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4740" uniqueCount="2673">
   <si>
     <t>var</t>
   </si>
@@ -8039,6 +8039,18 @@
   </si>
   <si>
     <t>toilet_clean_flies</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>kitchen</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>livestock</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>wealth_score</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -8470,8 +8482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -9560,6 +9572,12 @@
       <c r="B85" t="s">
         <v>158</v>
       </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>2670</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
@@ -9646,6 +9664,12 @@
       <c r="B92" t="s">
         <v>172</v>
       </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>2671</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
@@ -9755,6 +9779,12 @@
       </c>
       <c r="B105" t="s">
         <v>200</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>2672</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Still working through impacts of other changes on Digital.R
</commit_message>
<xml_diff>
--- a/Excel/hh_vars_tokeep.xlsx
+++ b/Excel/hh_vars_tokeep.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4740" uniqueCount="2673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4743" uniqueCount="2676">
   <si>
     <t>var</t>
   </si>
@@ -8051,6 +8051,18 @@
   </si>
   <si>
     <t>wealth_score</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>num_members</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ed_head</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>marital_head</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -8482,8 +8494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A414" workbookViewId="0">
+      <selection activeCell="C427" sqref="C427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -9355,6 +9367,12 @@
       <c r="B59" t="s">
         <v>23</v>
       </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2673</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
@@ -10885,7 +10903,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" t="s">
         <v>363</v>
       </c>
@@ -10893,7 +10911,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" t="s">
         <v>364</v>
       </c>
@@ -10901,7 +10919,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" t="s">
         <v>365</v>
       </c>
@@ -10909,7 +10927,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" t="s">
         <v>366</v>
       </c>
@@ -10917,7 +10935,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" t="s">
         <v>367</v>
       </c>
@@ -10925,7 +10943,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" t="s">
         <v>368</v>
       </c>
@@ -10933,7 +10951,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" t="s">
         <v>369</v>
       </c>
@@ -10941,7 +10959,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" t="s">
         <v>370</v>
       </c>
@@ -10949,7 +10967,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" t="s">
         <v>371</v>
       </c>
@@ -10957,7 +10975,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" t="s">
         <v>372</v>
       </c>
@@ -10965,15 +10983,21 @@
         <v>351</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" t="s">
         <v>373</v>
       </c>
       <c r="B251" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" t="s">
         <v>375</v>
       </c>
@@ -10981,7 +11005,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" t="s">
         <v>376</v>
       </c>
@@ -10989,7 +11013,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" t="s">
         <v>377</v>
       </c>
@@ -10997,7 +11021,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" t="s">
         <v>378</v>
       </c>
@@ -11005,7 +11029,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" t="s">
         <v>379</v>
       </c>
@@ -12293,7 +12317,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" t="s">
         <v>547</v>
       </c>
@@ -12301,7 +12325,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" t="s">
         <v>548</v>
       </c>
@@ -12309,7 +12333,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" t="s">
         <v>549</v>
       </c>
@@ -12317,7 +12341,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" t="s">
         <v>550</v>
       </c>
@@ -12325,7 +12349,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" t="s">
         <v>551</v>
       </c>
@@ -12333,7 +12357,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" t="s">
         <v>552</v>
       </c>
@@ -12341,7 +12365,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" t="s">
         <v>553</v>
       </c>
@@ -12349,7 +12373,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" t="s">
         <v>554</v>
       </c>
@@ -12357,7 +12381,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" t="s">
         <v>555</v>
       </c>
@@ -12365,7 +12389,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" t="s">
         <v>556</v>
       </c>
@@ -12373,15 +12397,21 @@
         <v>535</v>
       </c>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" t="s">
         <v>557</v>
       </c>
       <c r="B427" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C427">
+        <v>1</v>
+      </c>
+      <c r="D427" t="s">
+        <v>2675</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" t="s">
         <v>559</v>
       </c>
@@ -12389,7 +12419,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" t="s">
         <v>560</v>
       </c>
@@ -12397,7 +12427,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" t="s">
         <v>561</v>
       </c>
@@ -12405,7 +12435,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" t="s">
         <v>562</v>
       </c>
@@ -12413,7 +12443,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" t="s">
         <v>563</v>
       </c>

</xml_diff>